<commit_message>
Cambios en menu, y varios
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -1,27 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hamst\OneDrive\Escritorio\proyectoApprende-main\testeo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Asignaturas\8°Semestre\ANALISIS\proyectoApprende\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FB0B6F-F47D-4B4F-AEA8-BB3A1DD727B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8912AD7-CB71-4272-8C60-9AB21B17A4BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5490" yWindow="2625" windowWidth="17700" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -341,9 +340,15 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="54.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" customWidth="1"/>
+    <col min="5" max="5" width="32" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>

</xml_diff>